<commit_message>
realizada modificacion de remito pedida por admin depo
</commit_message>
<xml_diff>
--- a/remito_template.xlsx
+++ b/remito_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ftorres\OneDrive - INTRALOG ARGENTINA S.A\autopick\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intralogargentinasa-my.sharepoint.com/personal/ftorres_intralog_com_ar/Documents/autopick/rep/pickup_chk_generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF530B5-45EC-49E6-B61F-9EBA092F67E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{CCF530B5-45EC-49E6-B61F-9EBA092F67E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10BAC043-F81B-44D3-8D6B-AEFC5F25822D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -569,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,6 +619,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
     </row>
@@ -824,63 +825,13 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>